<commit_message>
Onderzoek frameworks is oude bestand
</commit_message>
<xml_diff>
--- a/Documentatie/onderzoek Front-end Framework/Onderzoek Frameworks.xlsx
+++ b/Documentatie/onderzoek Front-end Framework/Onderzoek Frameworks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2e13\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fda31a1c6f414f4a/I-Project Groep 15/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="8_{4C405DD6-9137-4F4C-8119-1363532083C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{021D65F9-8C44-4644-8B3D-62A72AF5407E}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="8_{4C405DD6-9137-4F4C-8119-1363532083C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{AC626D89-4B87-4730-9779-9DA2FA193945}"/>
   <bookViews>
-    <workbookView xWindow="12255" yWindow="2610" windowWidth="17280" windowHeight="8970" xr2:uid="{D60495F8-7E3E-4C77-B1AD-C8FC36D44B12}"/>
+    <workbookView xWindow="-28920" yWindow="525" windowWidth="29040" windowHeight="15840" xr2:uid="{D60495F8-7E3E-4C77-B1AD-C8FC36D44B12}"/>
   </bookViews>
   <sheets>
     <sheet name="Front-End" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
   <si>
     <t>Naam</t>
   </si>
@@ -61,6 +61,19 @@
     <t>https://www.slant.co/versus/504/520/~bootstrap_vs_semantic-ui</t>
   </si>
   <si>
+    <t>RethinkDB</t>
+  </si>
+  <si>
+    <t>Goed voor realtime Markplaats, Samenwerkende web- en mobiele apps</t>
+  </si>
+  <si>
+    <t>Primaire sleutels zijn beperkt tot 127 tekens.
+Secundaire indices slaan geen objecten of nullwaarden op. Zie secundaire indexen gebruiken voor meer informatie.</t>
+  </si>
+  <si>
+    <t>https://rethinkdb.com/</t>
+  </si>
+  <si>
     <t>Foundation</t>
   </si>
   <si>
@@ -112,6 +125,15 @@
     <t>https://getuikit.com/</t>
   </si>
   <si>
+    <t>WooCommerce</t>
+  </si>
+  <si>
+    <t>Werkt met plugins, kan met themes werken maar ook helemaal zelf te maken. Makkelijk voor ieder team lid te begrijpen. Ook mensen die BIM gaan doen kuch, </t>
+  </si>
+  <si>
+    <t>https://woocommerce.com/</t>
+  </si>
+  <si>
     <t>Skeleton</t>
   </si>
   <si>
@@ -136,7 +158,7 @@
     <t>op de site zelf staat heel veel informatie over hoe Materialize werkt. grote selectie van componets</t>
   </si>
   <si>
-    <t xml:space="preserve">geen support van flexbox, </t>
+    <t>geen support van flexbox, </t>
   </si>
   <si>
     <t>https://materializecss.com/</t>
@@ -146,25 +168,13 @@
   </si>
   <si>
     <t>Laravel</t>
-  </si>
-  <si>
-    <t>Responsive, lightweight, modulair</t>
-  </si>
-  <si>
-    <t>Bugs, geen spectaculair design, gebruikt geen flexbox</t>
-  </si>
-  <si>
-    <t>https://purecss.io/</t>
-  </si>
-  <si>
-    <t>CodeIgniter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,13 +200,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -244,38 +247,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -291,7 +293,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -590,10 +592,10 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="86.5703125" customWidth="1"/>
@@ -603,7 +605,7 @@
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -616,15 +618,17 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -633,147 +637,173 @@
       <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="8"/>
+        <v>17</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="10"/>
       <c r="D5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="11"/>
       <c r="D8" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="B11" s="11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
+      <c r="C11" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>36</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{3514B3AC-595C-4B2A-B659-2298429012EA}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{B7C58480-EA38-4E3B-A37D-1EA6B7BF5BE3}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{85E02371-E1E2-47AA-9D42-FDB85934C513}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{8431C6A2-A210-4FDB-BCE5-26B692874ED9}"/>
-    <hyperlink ref="E2" r:id="rId5" xr:uid="{19C84CB8-251B-40BC-B776-07849EB2DF5B}"/>
-    <hyperlink ref="D6" r:id="rId6" xr:uid="{DDA150A0-32BB-48BB-9501-65418E462C8C}"/>
-    <hyperlink ref="E6" r:id="rId7" xr:uid="{7616F590-83C0-42EB-9AE7-AC7C2255C1B0}"/>
-    <hyperlink ref="E4" r:id="rId8" xr:uid="{08CF8F9A-CAC8-48CF-8F7B-9E0557A4DA74}"/>
-    <hyperlink ref="D8" r:id="rId9" xr:uid="{56B82B49-5113-4EE9-BB18-84D5AD0B06EE}"/>
-    <hyperlink ref="F6" r:id="rId10" xr:uid="{0C59BD0D-1D1D-4A0D-A410-46FCCB38962E}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{7261142C-3AC6-4A9B-9263-B6A9318B2328}"/>
-    <hyperlink ref="E7" r:id="rId12" xr:uid="{9B34A4E9-51B5-4B9B-9D4F-165E3235BB79}"/>
-    <hyperlink ref="D11" r:id="rId13" xr:uid="{9EA5B766-5930-4537-8E4B-5F2401D098CB}"/>
-    <hyperlink ref="E11" r:id="rId14" xr:uid="{59B3ACDD-BE8D-4D68-95D8-B3A5ECB8A509}"/>
-    <hyperlink ref="D10" r:id="rId15" xr:uid="{02474885-08D6-4FEE-8B06-37E462DAA649}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{8B78F589-93FC-4090-9807-1024592918A6}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{85E02371-E1E2-47AA-9D42-FDB85934C513}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{8431C6A2-A210-4FDB-BCE5-26B692874ED9}"/>
+    <hyperlink ref="E2" r:id="rId6" xr:uid="{19C84CB8-251B-40BC-B776-07849EB2DF5B}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{DDA150A0-32BB-48BB-9501-65418E462C8C}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{7616F590-83C0-42EB-9AE7-AC7C2255C1B0}"/>
+    <hyperlink ref="E4" r:id="rId9" xr:uid="{08CF8F9A-CAC8-48CF-8F7B-9E0557A4DA74}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{56B82B49-5113-4EE9-BB18-84D5AD0B06EE}"/>
+    <hyperlink ref="F6" r:id="rId11" xr:uid="{0C59BD0D-1D1D-4A0D-A410-46FCCB38962E}"/>
+    <hyperlink ref="D8" r:id="rId12" xr:uid="{E6C90C7B-BC6D-461C-95F8-5CE41BEA0F22}"/>
+    <hyperlink ref="D9" r:id="rId13" xr:uid="{7261142C-3AC6-4A9B-9263-B6A9318B2328}"/>
+    <hyperlink ref="E9" r:id="rId14" xr:uid="{9B34A4E9-51B5-4B9B-9D4F-165E3235BB79}"/>
+    <hyperlink ref="D11" r:id="rId15" xr:uid="{9EA5B766-5930-4537-8E4B-5F2401D098CB}"/>
+    <hyperlink ref="E11" r:id="rId16" xr:uid="{59B3ACDD-BE8D-4D68-95D8-B3A5ECB8A509}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -781,20 +811,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00509AFA-B672-4F91-8384-D62CE6CDD48A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,14 +838,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>